<commit_message>
Loading submission sheet successfully
</commit_message>
<xml_diff>
--- a/AEF_files copy/11.syntax.failed/202405241221---AEF Guyana 2024 Revised 4 Final.syntax_checked.xlsx
+++ b/AEF_files copy/11.syntax.failed/202405241221---AEF Guyana 2024 Revised 4 Final.syntax_checked.xlsx
@@ -2137,8 +2137,8 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008FB6730B0802B54A9F00C78B857E1443" ma:contentTypeVersion="21" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e7d0671dbe340d15fdce5ab7e9f4c491">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="819ae873-75e1-413b-9d00-7af9258cf281" xmlns:ns3="eb4559c4-8463-4985-927f-f0d558bff8f0" xmlns:ns4="13d80b15-5f07-43ab-b435-85767a7dac08" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2feafd61044eb4abe44eb47c2e62f3e5" ns2:_="" ns3:_="" ns4:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008FB6730B0802B54A9F00C78B857E1443" ma:contentTypeVersion="21" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e758502e7902c92bdb050e89a8fea950">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="819ae873-75e1-413b-9d00-7af9258cf281" xmlns:ns3="eb4559c4-8463-4985-927f-f0d558bff8f0" xmlns:ns4="13d80b15-5f07-43ab-b435-85767a7dac08" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f4060acd4b29e25a8a76462245842ebf" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="819ae873-75e1-413b-9d00-7af9258cf281"/>
     <xsd:import namespace="eb4559c4-8463-4985-927f-f0d558bff8f0"/>
     <xsd:import namespace="13d80b15-5f07-43ab-b435-85767a7dac08"/>
@@ -2448,17 +2448,17 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1633A7C5-7197-4738-B475-E09F123471EE}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FB49CDCC-255A-4D07-84EC-870F3E2C6173}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6FBD7F3F-21E7-4429-B2D9-24EB6A4E7B5C}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{56804DAC-74DE-4BB3-BDB4-E6533F08EABC}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{03C25D36-2A6D-4EAB-8D40-6EE1A5237F14}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A97F33F5-A820-46BE-B555-9BBBB3E6A9E9}"/>
 </file>
 
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{28FFF3FE-2508-4DC7-A49C-120E7045559D}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{269B3436-C9D3-4299-ADA9-D7974850A10E}"/>
 </file>
</xml_diff>